<commit_message>
Uploading new graphs creating during lab.
</commit_message>
<xml_diff>
--- a/lab2_trees/avl_and_bst_graphs.xlsx
+++ b/lab2_trees/avl_and_bst_graphs.xlsx
@@ -5,23 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mateusz\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\mwasilew\sem2\AISDI\lab2\lab2_trees\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741BD145-02D8-42AE-AE4B-7EDA46B9ACDA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{024AADBB-AB54-42CE-AE71-D6194AB8FE9F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{2D05507F-BC4D-4F56-A993-0F288976D3C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Arkusz1!$A$3</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Arkusz1!$A$4</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Arkusz1!$B$2:$AX$2</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Arkusz1!$B$3:$AX$3</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Arkusz1!$B$4:$AX$4</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1318,6 +1311,21 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Arkusz1!$B$12:$AX$12</c:f>
@@ -5493,7 +5501,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF7A4D77-51AC-4AAA-989E-C5F11C1DD51C}">
   <dimension ref="A1:AX14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>

</xml_diff>